<commit_message>
nearly done with Part 1A
</commit_message>
<xml_diff>
--- a/adventures/ivywatch/monsters.xlsx
+++ b/adventures/ivywatch/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavin\Documents\drawsteel\_products\adventures\ivywatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDA5F5B-FF4D-4F5F-B062-34D76E9D8DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99685436-D313-49F8-AED1-33BDD6756962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="840" windowWidth="20475" windowHeight="13170" activeTab="2" xr2:uid="{918A4370-6BD2-4549-B40B-132AC3F5AF22}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="107">
   <si>
     <t>[Name]</t>
   </si>
@@ -507,29 +507,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Stamina </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Speed</t>
     </r>
     <r>
@@ -754,63 +731,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>8 poison damage; shift 2;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M&lt;2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bleeding</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -881,6 +801,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ---</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Distance</t>
     </r>
     <r>
@@ -986,6 +929,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1M / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Immunity</t>
     </r>
     <r>
@@ -996,7 +983,950 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> poison 2</t>
+      <t xml:space="preserve"> poison 3 / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Weakness </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fire 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Stamina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8 poison damage; shift 2;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M&lt;2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bleeding (save ends)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area, Magic</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All enemies in the burst</t>
+    </r>
+  </si>
+  <si>
+    <t>2 sonic damage</t>
+  </si>
+  <si>
+    <t>3 sonic damage</t>
+  </si>
+  <si>
+    <t>4 sonic damage</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 burst</t>
+    </r>
+  </si>
+  <si>
+    <t>Level 1 Retainer</t>
+  </si>
+  <si>
+    <t>Fey, Humanoid</t>
+  </si>
+  <si>
+    <t>Level 2 Leader</t>
+  </si>
+  <si>
+    <t>EV 16</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Stamina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>110</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Speed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Might 3   Agility 3   Reason 0   Intuition 0   Presence 3 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Vine Whip </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Action) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2d10 + 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Signature</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 creatures or objects</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8 poison damage; pull 1; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prone</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11 poison damage; pull 2; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prone</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">14 poison damage; pull 3; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prone</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> An ally targeted by this ability makes a free strike instead of taking damage (and takes no effect either).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Free Strike</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Yank the Leash </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Triggered Action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> One ally</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The ally becomes the target of the triggering strike instead.</t>
+    </r>
+  </si>
+  <si>
+    <t>End Effect</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Heel! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Maneuver)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Melee 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Each ally</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Slide each target 1 square.</t>
+    </r>
+  </si>
+  <si>
+    <t>Wode Houndmaster</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trigger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A creature targets the houndmaster with a strike.</t>
+    </r>
+  </si>
+  <si>
+    <t>At the end of their turn, the houndmaster can take 5 damage to end one save ends effect affecting them. This damage can’t be reduced in any way.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spore Bomb </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Villain Action 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3 Cube within 10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All enemies in area</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>toxic plant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grows in each space in the area and all targets are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M&lt;2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dazed (save ends).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sick 'Em! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Villain Action 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Self and 10 burst</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Self and all allies</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Each target moves up to their speed and makes a free strike.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Explosive Spores </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Villain Action 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ranged 10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Magic, Ranged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> One toxic plant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The target is destroyed. All toxic plants that are destroyed as a result of this ability explode. All creatures and objects within 1 burst of an exploding toxic plant take 3 fire damage.</t>
     </r>
   </si>
 </sst>
@@ -1004,7 +1934,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1047,6 +1977,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1181,7 +2118,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
@@ -1253,7 +2190,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1263,6 +2200,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1284,8 +2237,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD9D9D9"/>
       <color rgb="FFE5B8B7"/>
-      <color rgb="FFD9D9D9"/>
       <color rgb="FFFBD4B4"/>
       <color rgb="FFB6DDE8"/>
       <color rgb="FFD6E3BC"/>
@@ -1607,7 +2560,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2160,19 +3113,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF82A8B5-C780-4855-A5A0-A052A5BEE04A}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="3.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13">
       <c r="A1" s="33" t="s">
         <v>34</v>
       </c>
@@ -2183,8 +3138,18 @@
       </c>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2195,10 +3160,20 @@
       <c r="F2" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="5"/>
@@ -2207,236 +3182,660 @@
       <c r="F3" s="35" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="35"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="5"/>
       <c r="F4" s="35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>40</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="D9" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="H9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
       <c r="B13" s="39"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="H15" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="5" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="H16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="H17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="H18" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="H19" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="H20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="H21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="23" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="H22" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="H23" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="H24" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="H25" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="H28" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" customHeight="1">
+      <c r="H29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="H30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="H31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+    </row>
+    <row r="33" spans="8:13">
+      <c r="H33" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+    </row>
+    <row r="34" spans="8:13">
+      <c r="H34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="8:13">
+      <c r="H35" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+    </row>
+    <row r="36" spans="8:13" ht="15" customHeight="1">
+      <c r="H36" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+    </row>
+    <row r="37" spans="8:13">
+      <c r="H37" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+    </row>
+    <row r="38" spans="8:13">
+      <c r="H38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="8:13">
+      <c r="H39" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="L39" s="42"/>
+      <c r="M39" s="42"/>
+    </row>
+    <row r="40" spans="8:13" ht="15" customHeight="1">
+      <c r="H40" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+    </row>
+    <row r="41" spans="8:13">
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+    </row>
+    <row r="42" spans="8:13">
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="D20:F20"/>
+  <mergeCells count="46">
+    <mergeCell ref="H40:M42"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="H31:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H25:M27"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H13:M14"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F24"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F27"/>
+    <mergeCell ref="A20:F20"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A7:F7"/>
@@ -2445,6 +3844,7 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2452,12 +3852,287 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DFD280-CB3F-4A45-8F62-9CF1F8B27A7E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A22:F23"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:F10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>